<commit_message>
Optimize vector * vector^T multiplication
</commit_message>
<xml_diff>
--- a/benchmark/benchmark.xlsx
+++ b/benchmark/benchmark.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>Title</t>
   </si>
@@ -73,9 +73,6 @@
     <t>77594da</t>
   </si>
   <si>
-    <t>BLAS multiply matrix with a vector</t>
-  </si>
-  <si>
     <t>Speedup factor relative to previous</t>
   </si>
   <si>
@@ -85,19 +82,25 @@
     <t>934ce47</t>
   </si>
   <si>
-    <t>BLAS optimize matrix-vector multiplication with gramian (use symmetric functions)</t>
-  </si>
-  <si>
-    <t>BLAS optimize matrix-scalar multiplication</t>
-  </si>
-  <si>
     <t>3d3da72</t>
   </si>
   <si>
-    <t>BLAS optimize matrix-vector multiplication (multiply with scalar in one operation)</t>
-  </si>
-  <si>
     <t>d3226b2</t>
+  </si>
+  <si>
+    <t>Optimize mutiplication of vector with a transposed vector</t>
+  </si>
+  <si>
+    <t>Optimize matrix-vector multiplication (multiply with scalar in one operation)</t>
+  </si>
+  <si>
+    <t>Optimize matrix-scalar multiplication</t>
+  </si>
+  <si>
+    <t>Optimize matrix-vector multiplication with gramian (use symmetric functions)</t>
+  </si>
+  <si>
+    <t>Optimize matrix-vector multiplication</t>
   </si>
 </sst>
 </file>
@@ -519,8 +522,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="176" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView tabSelected="1" topLeftCell="B6" zoomScale="176" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -528,13 +531,13 @@
     <col min="1" max="1" width="19" customWidth="1"/>
     <col min="2" max="2" width="14.83203125" customWidth="1"/>
     <col min="3" max="3" width="12.6640625" customWidth="1"/>
-    <col min="5" max="5" width="11.1640625" customWidth="1"/>
-    <col min="6" max="6" width="19.1640625" customWidth="1"/>
+    <col min="5" max="6" width="12.5" customWidth="1"/>
     <col min="7" max="7" width="16.83203125" customWidth="1"/>
     <col min="8" max="8" width="19.5" customWidth="1"/>
+    <col min="9" max="9" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="8" customFormat="1" ht="84" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" s="8" customFormat="1" ht="108" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -542,24 +545,26 @@
         <v>2</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D1" s="9" t="s">
         <v>11</v>
       </c>
       <c r="E1" s="9" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="F1" s="9" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="G1" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="H1" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="I1" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="H1" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="I1" s="9"/>
       <c r="J1" s="9"/>
     </row>
     <row r="2" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -579,15 +584,17 @@
         <v>13</v>
       </c>
       <c r="F2" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G2" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="G2" s="4" t="s">
-        <v>20</v>
-      </c>
       <c r="H2" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="I2" s="4"/>
+        <v>18</v>
+      </c>
+      <c r="I2" s="4">
+        <v>686576</v>
+      </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
@@ -602,17 +609,20 @@
       <c r="D3" s="6">
         <v>2.2345250000000001</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="6">
         <v>2.3769640000000001</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="6">
         <v>1.6316999999999999</v>
       </c>
-      <c r="G3">
+      <c r="G3" s="6">
         <v>1.494346</v>
       </c>
-      <c r="H3">
+      <c r="H3" s="6">
         <v>1.498405</v>
+      </c>
+      <c r="I3" s="6">
+        <v>1.3208930000000001</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
@@ -625,17 +635,20 @@
       <c r="D4" s="6">
         <v>2.2342379999999999</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="6">
         <v>2.031304</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="6">
         <v>1.5724940000000001</v>
       </c>
-      <c r="G4">
+      <c r="G4" s="6">
         <v>1.41788</v>
       </c>
-      <c r="H4">
+      <c r="H4" s="6">
         <v>1.4025589999999999</v>
+      </c>
+      <c r="I4" s="6">
+        <v>1.3004560000000001</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
@@ -648,17 +661,20 @@
       <c r="D5" s="6">
         <v>2.3046340000000001</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="6">
         <v>2.1102750000000001</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="6">
         <v>1.5488200000000001</v>
       </c>
-      <c r="G5">
+      <c r="G5" s="6">
         <v>1.3958900000000001</v>
       </c>
-      <c r="H5">
+      <c r="H5" s="6">
         <v>1.3891290000000001</v>
+      </c>
+      <c r="I5" s="6">
+        <v>1.3263499999999999</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
@@ -671,17 +687,20 @@
       <c r="D6" s="6">
         <v>2.29678</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="6">
         <v>2.008524</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="6">
         <v>1.70242</v>
       </c>
-      <c r="G6">
+      <c r="G6" s="6">
         <v>1.395159</v>
       </c>
-      <c r="H6">
+      <c r="H6" s="6">
         <v>1.4478230000000001</v>
+      </c>
+      <c r="I6" s="6">
+        <v>1.3069580000000001</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
@@ -694,17 +713,20 @@
       <c r="D7" s="6">
         <v>2.2663720000000001</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="6">
         <v>2.2612480000000001</v>
       </c>
-      <c r="F7">
+      <c r="F7" s="6">
         <v>1.545174</v>
       </c>
-      <c r="G7">
+      <c r="G7" s="6">
         <v>1.4797180000000001</v>
       </c>
-      <c r="H7">
+      <c r="H7" s="6">
         <v>1.406212</v>
+      </c>
+      <c r="I7" s="6">
+        <v>1.224613</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
@@ -717,17 +739,20 @@
       <c r="D8" s="6">
         <v>2.4376030000000002</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="6">
         <v>2.1493570000000002</v>
       </c>
-      <c r="F8">
+      <c r="F8" s="6">
         <v>1.631364</v>
       </c>
-      <c r="G8">
+      <c r="G8" s="6">
         <v>1.3923639999999999</v>
       </c>
-      <c r="H8">
+      <c r="H8" s="6">
         <v>1.402091</v>
+      </c>
+      <c r="I8" s="6">
+        <v>1.249007</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
@@ -740,17 +765,20 @@
       <c r="D9" s="6">
         <v>2.3551160000000002</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="6">
         <v>2.1208520000000002</v>
       </c>
-      <c r="F9">
+      <c r="F9" s="6">
         <v>1.601618</v>
       </c>
-      <c r="G9">
+      <c r="G9" s="6">
         <v>1.4760949999999999</v>
       </c>
-      <c r="H9">
+      <c r="H9" s="6">
         <v>1.387365</v>
+      </c>
+      <c r="I9" s="6">
+        <v>1.2050160000000001</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
@@ -763,17 +791,20 @@
       <c r="D10" s="6">
         <v>2.2941929999999999</v>
       </c>
-      <c r="E10">
+      <c r="E10" s="6">
         <v>1.9968269999999999</v>
       </c>
-      <c r="F10">
+      <c r="F10" s="6">
         <v>1.574503</v>
       </c>
-      <c r="G10">
+      <c r="G10" s="6">
         <v>1.4029929999999999</v>
       </c>
-      <c r="H10">
+      <c r="H10" s="6">
         <v>1.488218</v>
+      </c>
+      <c r="I10" s="6">
+        <v>1.3269249999999999</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
@@ -786,17 +817,20 @@
       <c r="D11" s="6">
         <v>2.1960130000000002</v>
       </c>
-      <c r="E11">
+      <c r="E11" s="6">
         <v>2.1428210000000001</v>
       </c>
-      <c r="F11">
+      <c r="F11" s="6">
         <v>1.631643</v>
       </c>
-      <c r="G11">
+      <c r="G11" s="6">
         <v>1.4135070000000001</v>
       </c>
-      <c r="H11">
+      <c r="H11" s="6">
         <v>1.406965</v>
+      </c>
+      <c r="I11" s="6">
+        <v>1.2444280000000001</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
@@ -809,17 +843,20 @@
       <c r="D12" s="6">
         <v>2.2377750000000001</v>
       </c>
-      <c r="E12">
+      <c r="E12" s="6">
         <v>2.0271119999999998</v>
       </c>
-      <c r="F12">
+      <c r="F12" s="6">
         <v>1.6649449999999999</v>
       </c>
-      <c r="G12">
+      <c r="G12" s="6">
         <v>1.4011260000000001</v>
       </c>
-      <c r="H12">
+      <c r="H12" s="6">
         <v>1.393254</v>
+      </c>
+      <c r="I12" s="6">
+        <v>1.311685</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
@@ -858,6 +895,10 @@
         <f>AVERAGE(H3:H12)</f>
         <v>1.4222021</v>
       </c>
+      <c r="I14" s="6">
+        <f>AVERAGE(I3:I12)</f>
+        <v>1.2816330999999999</v>
+      </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
@@ -891,10 +932,14 @@
         <f>_xlfn.STDEV.S(H3:H12)/SQRT(COUNT(H3:H12))</f>
         <v>1.3014956245668549E-2</v>
       </c>
+      <c r="I15" s="6">
+        <f>_xlfn.STDEV.S(I3:I12)/SQRT(COUNT(I3:I12))</f>
+        <v>1.4553052219341779E-2</v>
+      </c>
     </row>
     <row r="16" spans="1:10" ht="32" x14ac:dyDescent="0.2">
       <c r="A16" s="10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B16" s="2"/>
       <c r="C16" s="2">
@@ -921,8 +966,12 @@
         <f>G14/H14</f>
         <v>1.0033087421260314</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" ht="32" x14ac:dyDescent="0.2">
+      <c r="I16" s="2">
+        <f>H14/I14</f>
+        <v>1.1096795955098226</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A17" s="10" t="s">
         <v>12</v>
       </c>
@@ -949,6 +998,10 @@
       <c r="H17" s="2">
         <f>$B$14/H14</f>
         <v>13.848888635447802</v>
+      </c>
+      <c r="I17" s="2">
+        <f>$B$14/I14</f>
+        <v>15.367829139244296</v>
       </c>
     </row>
   </sheetData>

</xml_diff>